<commit_message>
add urn to yaml variables of type urn
</commit_message>
<xml_diff>
--- a/tools/iso27001/mapping-iso27001-2022-to-iso27001-2013.xlsx
+++ b/tools/iso27001/mapping-iso27001-2022-to-iso27001-2013.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/iso27001/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8128A8A1-01A8-C542-9024-25F74E3821BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775C3BF4-D7F9-554E-8468-7EE4073FEDF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1948" uniqueCount="1190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1948" uniqueCount="1189">
   <si>
     <t>library_urn</t>
   </si>
@@ -3561,9 +3561,6 @@
   </si>
   <si>
     <t>Protection of information systems during audit testing</t>
-  </si>
-  <si>
-    <t>a7.6</t>
   </si>
   <si>
     <t>library_dependencies</t>
@@ -3953,8 +3950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="188" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="188" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4037,18 +4034,18 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B10" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B11" t="s">
         <v>1183</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1184</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -4077,23 +4074,23 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="B15" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="B16" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
@@ -4101,7 +4098,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
@@ -4112,10 +4109,10 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="C19" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
   </sheetData>
@@ -4127,8 +4124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E135"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" zoomScale="251" workbookViewId="0">
-      <selection activeCell="A106" sqref="A106:XFD107"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="251" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5127,7 +5124,7 @@
         <v>97</v>
       </c>
       <c r="B71" t="s">
-        <v>1178</v>
+        <v>1018</v>
       </c>
       <c r="C71" t="s">
         <v>172</v>

</xml_diff>